<commit_message>
Simplified the code base. Just run main.py
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bienstocke/Documents/Github/columnar-SBLAR-parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F3F0FE-A0D5-454D-BA36-8AE356D05F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE33358-A800-7140-AA70-2D27BF5926AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8620" yWindow="3900" windowWidth="60740" windowHeight="15700" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="valid" sheetId="1" r:id="rId1"/>
     <sheet name="invalid" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>uid</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>I LOVE THIS FIG!!!!!!!!!!</t>
+  </si>
+  <si>
+    <t>10BX939C5543TQA1133M3C</t>
   </si>
 </sst>
 </file>
@@ -664,7 +667,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -725,10 +728,10 @@
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B4" s="3">
-        <f t="shared" ref="B4:B11" si="0">B3+1</f>
+        <f t="shared" ref="B4:B8" si="0">B3+1</f>
         <v>20241003</v>
       </c>
       <c r="C4" s="1">

</xml_diff>

<commit_message>
451: add ct_guarantee and ct_guarantee_ff fields
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bienstocke/Documents/Github/columnar-SBLAR-parser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harjatia/Projects/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE33358-A800-7140-AA70-2D27BF5926AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C87306C-D1BC-624B-B09B-16C41B871235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8620" yWindow="3900" windowWidth="60740" windowHeight="15700" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
   <sheets>
     <sheet name="valid" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t>uid</t>
   </si>
@@ -97,6 +97,30 @@
   </si>
   <si>
     <t>10BX939C5543TQA1133M3C</t>
+  </si>
+  <si>
+    <t>1;2;3;4;5;6;7;8</t>
+  </si>
+  <si>
+    <t>ct_guarantee</t>
+  </si>
+  <si>
+    <t>1;2;3</t>
+  </si>
+  <si>
+    <t>10000;1200;1;2</t>
+  </si>
+  <si>
+    <t>ct_guarantee_ff</t>
+  </si>
+  <si>
+    <t>abc;def</t>
+  </si>
+  <si>
+    <t>1;2;3;4;5;6</t>
+  </si>
+  <si>
+    <t>977;1</t>
   </si>
 </sst>
 </file>
@@ -664,10 +688,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -677,10 +701,12 @@
     <col min="3" max="3" width="22.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="31.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="35.33203125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="19.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -696,8 +722,14 @@
       <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -710,8 +742,14 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -725,8 +763,14 @@
       <c r="D3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -740,8 +784,14 @@
       <c r="D4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -758,8 +808,14 @@
       <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -773,8 +829,14 @@
       <c r="D6" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F6" s="1">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -788,8 +850,11 @@
       <c r="D7" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -803,8 +868,11 @@
       <c r="D8" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F8" s="1">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -817,8 +885,14 @@
       <c r="D9" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F9" s="1">
+        <v>977</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -832,8 +906,14 @@
         <v>977</v>
       </c>
       <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -845,6 +925,12 @@
       </c>
       <c r="D11" s="1">
         <v>988</v>
+      </c>
+      <c r="F11" s="1">
+        <v>999</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated multi_value_field_restriction to include list of single vals. Made schema changes for credit_purpose_ff
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harjatia/Projects/pandera-parser-poc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcguffeej/Documents/Projects/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C87306C-D1BC-624B-B09B-16C41B871235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF52FCC2-8BAD-AC41-AD51-7F0383DB70B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
   <si>
     <t>uid</t>
   </si>
@@ -121,6 +121,21 @@
   </si>
   <si>
     <t>977;1</t>
+  </si>
+  <si>
+    <t>credit_purpose</t>
+  </si>
+  <si>
+    <t>credit_purpose_ff</t>
+  </si>
+  <si>
+    <t>1;1</t>
+  </si>
+  <si>
+    <t>1;988</t>
+  </si>
+  <si>
+    <t>def</t>
   </si>
 </sst>
 </file>
@@ -688,10 +703,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -703,10 +718,12 @@
     <col min="5" max="5" width="35.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="15.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -728,8 +745,14 @@
       <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -748,8 +771,14 @@
       <c r="G2" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -769,8 +798,14 @@
       <c r="G3" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H3" s="1">
+        <v>999</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -790,8 +825,14 @@
       <c r="G4" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -814,8 +855,14 @@
       <c r="G5" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -835,8 +882,14 @@
       <c r="G6" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H6" s="1">
+        <v>988</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -853,8 +906,11 @@
       <c r="F7" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -871,8 +927,11 @@
       <c r="F8" s="1">
         <v>977</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H8" s="1">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -891,8 +950,14 @@
       <c r="G9" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H9" s="1">
+        <v>977</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -903,7 +968,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="1">
-        <v>977</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="1" t="s">
@@ -912,8 +977,14 @@
       <c r="G10" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -924,12 +995,18 @@
         <v>4</v>
       </c>
       <c r="D11" s="1">
-        <v>988</v>
+        <v>10</v>
       </c>
       <c r="F11" s="1">
         <v>999</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
deleted old branch for task 450, pulled master, recreated branch and added ct_loan_term_and_flag in order to avoid merge conflict because of using Aldrian's conditional_field_conflict function before his branch was even merged with the main branch.
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harjatia/Projects/pandera-parser-poc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sultanin/Workspace/git/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C87306C-D1BC-624B-B09B-16C41B871235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDBF3DA-72AA-974A-AAC0-2D19E28C55DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>uid</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>977;1</t>
+  </si>
+  <si>
+    <t>ct_loan_term_flag</t>
+  </si>
+  <si>
+    <t>ct_loan_term</t>
   </si>
 </sst>
 </file>
@@ -688,10 +694,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -706,7 +712,7 @@
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -728,8 +734,14 @@
       <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -748,8 +760,14 @@
       <c r="G2" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H2" s="1">
+        <v>900</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -769,8 +787,14 @@
       <c r="G3" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H3" s="1">
+        <v>900</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -790,8 +814,14 @@
       <c r="G4" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H4" s="1">
+        <v>900</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -814,8 +844,14 @@
       <c r="G5" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H5" s="1">
+        <v>900</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -835,8 +871,14 @@
       <c r="G6" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H6" s="1">
+        <v>900</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -853,8 +895,11 @@
       <c r="F7" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -871,8 +916,14 @@
       <c r="F8" s="1">
         <v>977</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H8" s="1">
+        <v>988</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -891,8 +942,14 @@
       <c r="G9" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H9" s="1">
+        <v>999</v>
+      </c>
+      <c r="I9" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -912,8 +969,11 @@
       <c r="G10" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="H10" s="1">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -931,6 +991,9 @@
       </c>
       <c r="G11" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="H11" s="1">
+        <v>999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated xlsx file to resolve main merge issue
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcguffeej/Documents/Projects/pandera-parser-poc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harjatia/Projects/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF52FCC2-8BAD-AC41-AD51-7F0383DB70B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32294A45-592E-B749-8AA0-0EE0DEDC77B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>uid</t>
   </si>
@@ -123,19 +123,7 @@
     <t>977;1</t>
   </si>
   <si>
-    <t>credit_purpose</t>
-  </si>
-  <si>
-    <t>credit_purpose_ff</t>
-  </si>
-  <si>
-    <t>1;1</t>
-  </si>
-  <si>
-    <t>1;988</t>
-  </si>
-  <si>
-    <t>def</t>
+    <t>action_taken</t>
   </si>
 </sst>
 </file>
@@ -703,10 +691,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -718,12 +706,10 @@
     <col min="5" max="5" width="35.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -748,11 +734,8 @@
       <c r="H1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -771,14 +754,11 @@
       <c r="G2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -799,13 +779,10 @@
         <v>25</v>
       </c>
       <c r="H3" s="1">
-        <v>999</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -825,14 +802,11 @@
       <c r="G4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="H4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -855,14 +829,11 @@
       <c r="G5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="H5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -883,13 +854,10 @@
         <v>25</v>
       </c>
       <c r="H6" s="1">
-        <v>988</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -906,11 +874,11 @@
       <c r="F7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="H7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -928,10 +896,10 @@
         <v>977</v>
       </c>
       <c r="H8" s="1">
-        <v>977</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -951,13 +919,10 @@
         <v>25</v>
       </c>
       <c r="H9" s="1">
-        <v>977</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -968,7 +933,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="1">
-        <v>9</v>
+        <v>977</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="1" t="s">
@@ -977,14 +942,11 @@
       <c r="G10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="H10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -995,18 +957,12 @@
         <v>4</v>
       </c>
       <c r="D11" s="1">
-        <v>10</v>
+        <v>988</v>
       </c>
       <c r="F11" s="1">
         <v>999</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="1" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deleted older branch; pulled master, recreated the branch and added the changes
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harjatia/Projects/pandera-parser-poc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sultanin/Workspace/git/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32294A45-592E-B749-8AA0-0EE0DEDC77B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B90A751-EEE3-0246-A808-0DE8A5CD2EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>uid</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>action_taken</t>
+  </si>
+  <si>
+    <t>app_recipient</t>
   </si>
 </sst>
 </file>
@@ -691,10 +694,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -709,7 +712,7 @@
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -734,8 +737,11 @@
       <c r="H1" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -757,8 +763,11 @@
       <c r="H2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -781,8 +790,11 @@
       <c r="H3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -805,8 +817,11 @@
       <c r="H4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -832,8 +847,11 @@
       <c r="H5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -856,8 +874,11 @@
       <c r="H6" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -877,8 +898,11 @@
       <c r="H7" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -899,7 +923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -921,8 +945,11 @@
       <c r="H9" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -945,8 +972,11 @@
       <c r="H10" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I10" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Cleaned up data type logic in multi_value_field_restriction()
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sultanin/Workspace/git/pandera-parser-poc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcguffeej/Documents/Projects/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B90A751-EEE3-0246-A808-0DE8A5CD2EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B1B5B3-E1EF-F24D-ACD0-1CA60740CF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
   <si>
     <t>uid</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>app_recipient</t>
+  </si>
+  <si>
+    <t>credit_purpose</t>
+  </si>
+  <si>
+    <t>credit_purpose_ff</t>
+  </si>
+  <si>
+    <t>1;999</t>
   </si>
 </sst>
 </file>
@@ -694,10 +703,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -709,10 +718,11 @@
     <col min="5" max="5" width="35.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="14.5" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -735,13 +745,19 @@
         <v>24</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -760,14 +776,20 @@
       <c r="G2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="1">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="H2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -788,13 +810,19 @@
         <v>25</v>
       </c>
       <c r="H3" s="1">
-        <v>2</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>988</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="1">
+        <v>2</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -814,14 +842,20 @@
       <c r="G4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="1">
         <v>3</v>
       </c>
-      <c r="I4" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -844,14 +878,20 @@
       <c r="G5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="1">
         <v>4</v>
       </c>
-      <c r="I5" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -871,14 +911,20 @@
       <c r="G6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="1">
         <v>5</v>
       </c>
-      <c r="I6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -895,14 +941,17 @@
       <c r="F7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="1">
         <v>6</v>
       </c>
-      <c r="I7" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="K7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -920,10 +969,13 @@
         <v>977</v>
       </c>
       <c r="H8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>977</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -943,13 +995,19 @@
         <v>25</v>
       </c>
       <c r="H9" s="1">
-        <v>2</v>
-      </c>
-      <c r="I9" s="1">
+        <v>977</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2</v>
+      </c>
+      <c r="K9" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -969,14 +1027,20 @@
       <c r="G10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="1">
         <v>3</v>
       </c>
-      <c r="I10" s="1">
+      <c r="K10" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -993,6 +1057,12 @@
         <v>999</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="1">
+        <v>999</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added date_in_range() and added check to action_taken_date
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcguffeej/Documents/Projects/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B1B5B3-E1EF-F24D-ACD0-1CA60740CF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991D34D9-8E2C-AA47-9C5B-CACC47E54E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
   <si>
     <t>uid</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>1;999</t>
+  </si>
+  <si>
+    <t>action_taken_date</t>
   </si>
 </sst>
 </file>
@@ -703,10 +706,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -719,10 +722,13 @@
     <col min="6" max="6" width="19.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.5" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="13" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -754,10 +760,13 @@
         <v>28</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -785,11 +794,14 @@
       <c r="J2" s="1">
         <v>1</v>
       </c>
-      <c r="K2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="K2" s="3">
+        <v>20241001</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -818,11 +830,15 @@
       <c r="J3" s="1">
         <v>2</v>
       </c>
-      <c r="K3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="K3" s="3">
+        <f>K2+1</f>
+        <v>20241002</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -851,11 +867,15 @@
       <c r="J4" s="1">
         <v>3</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="3">
+        <f t="shared" ref="K4:K8" si="1">K3+1</f>
+        <v>20241003</v>
+      </c>
+      <c r="L4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -887,11 +907,15 @@
       <c r="J5" s="1">
         <v>4</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="3">
+        <f t="shared" si="1"/>
+        <v>20241004</v>
+      </c>
+      <c r="L5" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -920,11 +944,15 @@
       <c r="J6" s="1">
         <v>5</v>
       </c>
-      <c r="K6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="K6" s="3">
+        <f t="shared" si="1"/>
+        <v>20241005</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -947,11 +975,14 @@
       <c r="J7" s="1">
         <v>6</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="3">
+        <v>20250106</v>
+      </c>
+      <c r="L7" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -974,8 +1005,11 @@
       <c r="J8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="K8" s="3">
+        <v>20240907</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1003,11 +1037,14 @@
       <c r="J9" s="1">
         <v>2</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="4">
+        <v>20241433</v>
+      </c>
+      <c r="L9" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1036,11 +1073,14 @@
       <c r="J10" s="1">
         <v>3</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="4">
+        <v>2021010</v>
+      </c>
+      <c r="L10" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1064,6 +1104,9 @@
       </c>
       <c r="I11" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed date logic to include the start and end dates in the accepted range
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcguffeej/Documents/Projects/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991D34D9-8E2C-AA47-9C5B-CACC47E54E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF084FAC-41FC-3349-8F1D-6DA68340F093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -709,7 +709,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -945,8 +945,7 @@
         <v>5</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" si="1"/>
-        <v>20241005</v>
+        <v>20241231</v>
       </c>
       <c r="L6" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Updated method names to match the FIG
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcguffeej/Documents/Projects/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF084FAC-41FC-3349-8F1D-6DA68340F093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6039785E-6260-1945-AE0F-C593D7E76E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -709,7 +709,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -868,7 +868,7 @@
         <v>3</v>
       </c>
       <c r="K4" s="3">
-        <f t="shared" ref="K4:K8" si="1">K3+1</f>
+        <f t="shared" ref="K4:K5" si="1">K3+1</f>
         <v>20241003</v>
       </c>
       <c r="L4" s="1">

</xml_diff>

<commit_message>
WIP: Added tentative date_value_conflict() function. Added docstrings for this and invalid_date_value() function
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcguffeej/Documents/Projects/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6039785E-6260-1945-AE0F-C593D7E76E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F791A6E1-AAF8-8842-9A99-5EB5A7AD6522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
   <sheets>
     <sheet name="valid" sheetId="1" r:id="rId1"/>
@@ -708,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -806,8 +806,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3">
-        <f>B2+1</f>
-        <v>20241002</v>
+        <v>20241001</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -844,7 +843,7 @@
       </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B8" si="0">B3+1</f>
-        <v>20241003</v>
+        <v>20241002</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
@@ -881,7 +880,7 @@
       </c>
       <c r="B5" s="3">
         <f t="shared" si="0"/>
-        <v>20241004</v>
+        <v>20241003</v>
       </c>
       <c r="C5" s="2">
         <v>5</v>
@@ -921,7 +920,7 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" si="0"/>
-        <v>20241005</v>
+        <v>20241004</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -957,7 +956,7 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" si="0"/>
-        <v>20241006</v>
+        <v>20241005</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -987,7 +986,7 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" si="0"/>
-        <v>20241007</v>
+        <v>20241006</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Task 460, amount_applied_for and flag
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harjatia/Projects/pandera-parser-poc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sultanin/Workspace/git/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E3630D-73D5-9A42-B75C-BBA5AAD44C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C169AF3F-9C6C-1644-AA75-3BD22177FB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="37">
   <si>
     <t>uid</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>abc</t>
+  </si>
+  <si>
+    <t>amount_applied_for_flag</t>
+  </si>
+  <si>
+    <t>amount_applied_for</t>
   </si>
 </sst>
 </file>
@@ -709,10 +715,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -730,7 +736,7 @@
     <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -767,8 +773,14 @@
       <c r="L1" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -802,8 +814,14 @@
       <c r="L2" s="1">
         <v>1000</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M2">
+        <v>900</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -838,8 +856,12 @@
       <c r="L3" s="1">
         <v>1000</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <v>988</v>
+      </c>
+      <c r="N3"/>
+    </row>
+    <row r="4" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -871,8 +893,12 @@
       <c r="K4" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M4">
+        <v>999</v>
+      </c>
+      <c r="N4"/>
+    </row>
+    <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -910,8 +936,12 @@
       <c r="L5" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M5"/>
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -946,8 +976,14 @@
       <c r="L6" s="1">
         <v>1000</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M6">
+        <v>988</v>
+      </c>
+      <c r="N6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -973,8 +1009,14 @@
       <c r="K7" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M7">
+        <v>999</v>
+      </c>
+      <c r="N7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1000,8 +1042,14 @@
       <c r="L8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M8">
+        <v>900</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1035,8 +1083,14 @@
       <c r="L9" s="1">
         <v>1000</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M9">
+        <v>900</v>
+      </c>
+      <c r="N9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1071,8 +1125,12 @@
       <c r="L10" s="1">
         <v>1000</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="M10">
+        <v>900</v>
+      </c>
+      <c r="N10"/>
+    </row>
+    <row r="11" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1099,6 +1157,10 @@
       </c>
       <c r="L11" s="1">
         <v>1000</v>
+      </c>
+      <c r="M11"/>
+      <c r="N11">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add validations for denial_reasons and denial_reasons_ff fields (#14)
Add validation(s) for denial_reasons and denial_reasons_ff fields. These include:
denial_reasons.invalid_enum_value
denial_reasons.invalid_number_of_values
denial_reasons_ff.invalid_text_length
denial_reasons.enum_value_conflict
denial_reasons_ff.conditional_field_conflict
denial_reasons.multi_value_field_restriction
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcguffeej/Documents/Projects/pandera-parser-poc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harjatia/Projects/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A60AEA6-F083-F74F-83E6-622AE339965B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8265FCB-F173-C546-8016-724E0C24187F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
   <si>
     <t>uid</t>
   </si>
@@ -150,7 +150,22 @@
     <t>amount_applied_for</t>
   </si>
   <si>
-    <t>action_taken_date</t>
+    <t>denial_reasons</t>
+  </si>
+  <si>
+    <t>denial_reasons_ff</t>
+  </si>
+  <si>
+    <t>1;2;999</t>
+  </si>
+  <si>
+    <t>1;2;3;101;4</t>
+  </si>
+  <si>
+    <t>abc123</t>
+  </si>
+  <si>
+    <t>1;3;4;999</t>
   </si>
 </sst>
 </file>
@@ -718,10 +733,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -734,13 +749,12 @@
     <col min="6" max="6" width="19.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.5" style="1" customWidth="1"/>
-    <col min="9" max="10" width="10.83203125" style="1"/>
-    <col min="11" max="11" width="13.83203125" style="1" customWidth="1"/>
+    <col min="9" max="11" width="10.83203125" style="1"/>
     <col min="12" max="12" width="19" style="1" customWidth="1"/>
     <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -772,22 +786,25 @@
         <v>28</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="P1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -815,23 +832,24 @@
       <c r="J2" s="1">
         <v>1</v>
       </c>
-      <c r="K2" s="3">
-        <v>20241001</v>
+      <c r="K2" s="1">
+        <v>1</v>
       </c>
       <c r="L2" s="1">
-        <v>1</v>
-      </c>
-      <c r="M2" s="1">
         <v>1000</v>
       </c>
+      <c r="M2">
+        <v>900</v>
+      </c>
       <c r="N2">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P2"/>
+    </row>
+    <row r="3" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -860,22 +878,22 @@
       <c r="J3" s="1">
         <v>2</v>
       </c>
-      <c r="K3" s="3">
-        <f>K2+1</f>
-        <v>20241002</v>
+      <c r="K3" s="1">
+        <v>1</v>
       </c>
       <c r="L3" s="1">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1">
         <v>1000</v>
       </c>
-      <c r="N3">
+      <c r="M3">
         <v>988</v>
       </c>
-      <c r="O3"/>
-    </row>
-    <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="N3"/>
+      <c r="O3">
+        <v>101</v>
+      </c>
+      <c r="P3"/>
+    </row>
+    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -904,19 +922,19 @@
       <c r="J4" s="1">
         <v>3</v>
       </c>
-      <c r="K4" s="3">
-        <f t="shared" ref="K4:K5" si="1">K3+1</f>
-        <v>20241003</v>
-      </c>
-      <c r="L4" s="1">
+      <c r="K4" s="1">
         <v>2</v>
       </c>
-      <c r="N4">
+      <c r="M4">
         <v>999</v>
       </c>
-      <c r="O4"/>
-    </row>
-    <row r="5" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="N4"/>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4"/>
+    </row>
+    <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -948,22 +966,22 @@
       <c r="J5" s="1">
         <v>4</v>
       </c>
-      <c r="K5" s="3">
-        <f t="shared" si="1"/>
-        <v>20241004</v>
-      </c>
-      <c r="L5" s="1">
+      <c r="K5" s="1">
         <v>2</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N5"/>
+      <c r="M5"/>
+      <c r="N5">
+        <v>1</v>
+      </c>
       <c r="O5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="P5"/>
+    </row>
+    <row r="6" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -992,23 +1010,24 @@
       <c r="J6" s="1">
         <v>5</v>
       </c>
-      <c r="K6" s="3">
-        <v>20241231</v>
+      <c r="K6" s="1">
+        <v>1</v>
       </c>
       <c r="L6" s="1">
-        <v>1</v>
-      </c>
-      <c r="M6" s="1">
         <v>1000</v>
       </c>
+      <c r="M6">
+        <v>988</v>
+      </c>
       <c r="N6">
-        <v>988</v>
-      </c>
-      <c r="O6">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="O6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6"/>
+    </row>
+    <row r="7" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1031,20 +1050,21 @@
       <c r="J7" s="1">
         <v>6</v>
       </c>
-      <c r="K7" s="3">
-        <v>20280106</v>
-      </c>
-      <c r="L7" s="1">
+      <c r="K7" s="1">
         <v>2</v>
       </c>
+      <c r="M7">
+        <v>999</v>
+      </c>
       <c r="N7">
+        <v>20</v>
+      </c>
+      <c r="O7">
         <v>999</v>
       </c>
-      <c r="O7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="P7"/>
+    </row>
+    <row r="8" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1067,20 +1087,21 @@
       <c r="J8" s="1">
         <v>1</v>
       </c>
-      <c r="K8" s="3">
-        <v>20240907</v>
-      </c>
-      <c r="M8" s="1">
+      <c r="L8" s="1">
         <v>0</v>
       </c>
+      <c r="M8">
+        <v>900</v>
+      </c>
       <c r="N8">
-        <v>900</v>
-      </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="O8" t="s">
+        <v>40</v>
+      </c>
+      <c r="P8"/>
+    </row>
+    <row r="9" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1108,23 +1129,26 @@
       <c r="J9" s="1">
         <v>2</v>
       </c>
-      <c r="K9" s="4">
-        <v>20241433</v>
+      <c r="K9" s="1">
+        <v>3</v>
       </c>
       <c r="L9" s="1">
-        <v>3</v>
-      </c>
-      <c r="M9" s="1">
         <v>1000</v>
       </c>
+      <c r="M9">
+        <v>900</v>
+      </c>
       <c r="N9">
-        <v>900</v>
+        <v>30</v>
       </c>
       <c r="O9">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="P9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1153,21 +1177,22 @@
       <c r="J10" s="1">
         <v>3</v>
       </c>
-      <c r="K10" s="4">
-        <v>2021010</v>
+      <c r="K10" s="1">
+        <v>5</v>
       </c>
       <c r="L10" s="1">
-        <v>5</v>
-      </c>
-      <c r="M10" s="1">
         <v>1000</v>
       </c>
-      <c r="N10">
+      <c r="M10">
         <v>900</v>
       </c>
-      <c r="O10"/>
-    </row>
-    <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="N10"/>
+      <c r="O10" t="s">
+        <v>42</v>
+      </c>
+      <c r="P10"/>
+    </row>
+    <row r="11" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1192,16 +1217,17 @@
       <c r="I11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M11" s="1">
+      <c r="L11" s="1">
         <v>1000</v>
       </c>
-      <c r="N11"/>
+      <c r="M11"/>
+      <c r="N11">
+        <v>20</v>
+      </c>
       <c r="O11">
-        <v>20</v>
-      </c>
+        <v>977</v>
+      </c>
+      <c r="P11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ticket 526 add pricing_pricing_interest_rate_type field
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harjatia/Projects/pandera-parser-poc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sultanin/Workspace/git/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8265FCB-F173-C546-8016-724E0C24187F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FD90A3-4AF1-6D4E-9F13-798FD05ED089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
   <si>
     <t>uid</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>1;3;4;999</t>
+  </si>
+  <si>
+    <t>pricing_interest_rate_type</t>
   </si>
 </sst>
 </file>
@@ -733,10 +736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -751,10 +754,13 @@
     <col min="8" max="8" width="14.5" style="1" customWidth="1"/>
     <col min="9" max="11" width="10.83203125" style="1"/>
     <col min="12" max="12" width="19" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="13" max="16" width="10.83203125" style="1"/>
+    <col min="17" max="17" width="22.33203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14.83203125" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -803,8 +809,12 @@
       <c r="P1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1"/>
+    </row>
+    <row r="2" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -848,8 +858,12 @@
         <v>1</v>
       </c>
       <c r="P2"/>
-    </row>
-    <row r="3" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2"/>
+    </row>
+    <row r="3" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -892,8 +906,12 @@
         <v>101</v>
       </c>
       <c r="P3"/>
-    </row>
-    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3"/>
+    </row>
+    <row r="4" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -933,8 +951,12 @@
         <v>1</v>
       </c>
       <c r="P4"/>
-    </row>
-    <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q4">
+        <v>3</v>
+      </c>
+      <c r="R4"/>
+    </row>
+    <row r="5" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -980,8 +1002,12 @@
         <v>102</v>
       </c>
       <c r="P5"/>
-    </row>
-    <row r="6" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q5">
+        <v>4</v>
+      </c>
+      <c r="R5"/>
+    </row>
+    <row r="6" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1026,8 +1052,12 @@
         <v>39</v>
       </c>
       <c r="P6"/>
-    </row>
-    <row r="7" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6"/>
+    </row>
+    <row r="7" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1063,8 +1093,12 @@
         <v>999</v>
       </c>
       <c r="P7"/>
-    </row>
-    <row r="8" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q7">
+        <v>6</v>
+      </c>
+      <c r="R7"/>
+    </row>
+    <row r="8" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1100,8 +1134,12 @@
         <v>40</v>
       </c>
       <c r="P8"/>
-    </row>
-    <row r="9" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q8">
+        <v>999</v>
+      </c>
+      <c r="R8"/>
+    </row>
+    <row r="9" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1147,8 +1185,12 @@
       <c r="P9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9"/>
+    </row>
+    <row r="10" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1191,8 +1233,12 @@
         <v>42</v>
       </c>
       <c r="P10"/>
-    </row>
-    <row r="11" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q10">
+        <v>10</v>
+      </c>
+      <c r="R10"/>
+    </row>
+    <row r="11" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1228,6 +1274,10 @@
         <v>977</v>
       </c>
       <c r="P11"/>
+      <c r="Q11">
+        <v>1000</v>
+      </c>
+      <c r="R11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ticket 527, add pricing_init_rate_period field
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harjatia/Projects/pandera-parser-poc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sultanin/Workspace/git/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8265FCB-F173-C546-8016-724E0C24187F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A0E86B-2EE7-9045-9D1E-5FF5FF068522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
   <si>
     <t>uid</t>
   </si>
@@ -166,6 +166,21 @@
   </si>
   <si>
     <t>1;3;4;999</t>
+  </si>
+  <si>
+    <t>pricing_interest_rate_type</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>pricing_init_rate_period</t>
   </si>
 </sst>
 </file>
@@ -733,10 +748,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -754,7 +769,7 @@
     <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -803,8 +818,14 @@
       <c r="P1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -848,8 +869,14 @@
         <v>1</v>
       </c>
       <c r="P2"/>
-    </row>
-    <row r="3" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -892,8 +919,14 @@
         <v>101</v>
       </c>
       <c r="P3"/>
-    </row>
-    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q3" s="1">
+        <v>2</v>
+      </c>
+      <c r="R3" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -933,8 +966,14 @@
         <v>1</v>
       </c>
       <c r="P4"/>
-    </row>
-    <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q4" s="1">
+        <v>3</v>
+      </c>
+      <c r="R4" s="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -980,8 +1019,14 @@
         <v>102</v>
       </c>
       <c r="P5"/>
-    </row>
-    <row r="6" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q5" s="1">
+        <v>4</v>
+      </c>
+      <c r="R5" s="1">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1026,8 +1071,14 @@
         <v>39</v>
       </c>
       <c r="P6"/>
-    </row>
-    <row r="7" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q6" s="1">
+        <v>5</v>
+      </c>
+      <c r="R6" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1063,8 +1114,14 @@
         <v>999</v>
       </c>
       <c r="P7"/>
-    </row>
-    <row r="8" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q7" s="1">
+        <v>6</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1100,8 +1157,14 @@
         <v>40</v>
       </c>
       <c r="P8"/>
-    </row>
-    <row r="9" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q8" s="1">
+        <v>7</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1147,8 +1210,14 @@
       <c r="P9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q9" s="1">
+        <v>900</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1191,8 +1260,14 @@
         <v>42</v>
       </c>
       <c r="P10"/>
-    </row>
-    <row r="11" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q10" s="1">
+        <v>1</v>
+      </c>
+      <c r="R10" s="1">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1228,6 +1303,12 @@
         <v>977</v>
       </c>
       <c r="P11"/>
+      <c r="Q11" s="1">
+        <v>3</v>
+      </c>
+      <c r="R11" s="1">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Renamed invalid numeric function to reflect more accurately. Added logic for handling decimals
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcguffeej/Documents/Projects/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B21F41-7DF1-2A4B-A8C0-11819A3D944D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D7554F-F1CC-1D4D-A3F7-A2306355B15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -742,7 +742,7 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Task 537: add pricing_prepenalty_allowed and pricing_prepenalty_exists fields
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harjatia/Projects/pandera-parser-poc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sultanin/Workspace/git/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8265FCB-F173-C546-8016-724E0C24187F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FD6679-DA64-E141-A737-B0C39EE0D801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
+    <workbookView xWindow="0" yWindow="5640" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
   <sheets>
     <sheet name="valid" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="45">
   <si>
     <t>uid</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>1;3;4;999</t>
+  </si>
+  <si>
+    <t>pricing_prepenalty_allowed</t>
+  </si>
+  <si>
+    <t>pricing_prepenalty_exists</t>
   </si>
 </sst>
 </file>
@@ -733,10 +739,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -754,7 +760,7 @@
     <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -803,8 +809,14 @@
       <c r="P1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -848,8 +860,14 @@
         <v>1</v>
       </c>
       <c r="P2"/>
-    </row>
-    <row r="3" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -892,8 +910,14 @@
         <v>101</v>
       </c>
       <c r="P3"/>
-    </row>
-    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q3" s="1">
+        <v>2</v>
+      </c>
+      <c r="R3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -933,8 +957,14 @@
         <v>1</v>
       </c>
       <c r="P4"/>
-    </row>
-    <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q4" s="1">
+        <v>999</v>
+      </c>
+      <c r="R4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -980,8 +1010,14 @@
         <v>102</v>
       </c>
       <c r="P5"/>
-    </row>
-    <row r="6" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1026,8 +1062,14 @@
         <v>39</v>
       </c>
       <c r="P6"/>
-    </row>
-    <row r="7" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q6" s="1">
+        <v>3</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1063,8 +1105,14 @@
         <v>999</v>
       </c>
       <c r="P7"/>
-    </row>
-    <row r="8" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q7" s="1">
+        <v>1</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1100,8 +1148,14 @@
         <v>40</v>
       </c>
       <c r="P8"/>
-    </row>
-    <row r="9" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q8" s="1">
+        <v>2</v>
+      </c>
+      <c r="R8" s="1">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1147,8 +1201,14 @@
       <c r="P9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q9" s="1">
+        <v>999</v>
+      </c>
+      <c r="R9" s="1">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1191,8 +1251,14 @@
         <v>42</v>
       </c>
       <c r="P10"/>
-    </row>
-    <row r="11" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q10" s="1">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1228,6 +1294,12 @@
         <v>977</v>
       </c>
       <c r="P11"/>
+      <c r="Q11" s="1">
+        <v>0</v>
+      </c>
+      <c r="R11" s="1">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added more validations and corrected naming for valid numeric format
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sultanin/Workspace/git/pandera-parser-poc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcguffeej/Documents/Projects/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FD90A3-4AF1-6D4E-9F13-798FD05ED089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A949E291-EC82-A94C-BFE0-76E5661748B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
   <si>
     <t>uid</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>pricing_interest_rate_type</t>
+  </si>
+  <si>
+    <t>pricing_fixed_rate</t>
   </si>
 </sst>
 </file>
@@ -736,10 +739,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="S1" sqref="S1:S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -760,7 +763,7 @@
     <col min="19" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -812,9 +815,14 @@
       <c r="Q1" t="s">
         <v>43</v>
       </c>
-      <c r="R1"/>
-    </row>
-    <row r="2" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="R1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -861,9 +869,14 @@
       <c r="Q2">
         <v>1</v>
       </c>
-      <c r="R2"/>
-    </row>
-    <row r="3" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="R2" s="1">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -909,9 +922,14 @@
       <c r="Q3">
         <v>2</v>
       </c>
-      <c r="R3"/>
-    </row>
-    <row r="4" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="R3" s="1">
+        <v>2</v>
+      </c>
+      <c r="S3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -954,9 +972,14 @@
       <c r="Q4">
         <v>3</v>
       </c>
-      <c r="R4"/>
-    </row>
-    <row r="5" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="R4" s="1">
+        <v>2</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1005,9 +1028,14 @@
       <c r="Q5">
         <v>4</v>
       </c>
-      <c r="R5"/>
-    </row>
-    <row r="6" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="R5" s="1">
+        <v>3</v>
+      </c>
+      <c r="S5">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1055,9 +1083,14 @@
       <c r="Q6">
         <v>5</v>
       </c>
-      <c r="R6"/>
-    </row>
-    <row r="7" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="R6" s="1">
+        <v>4</v>
+      </c>
+      <c r="S6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1096,9 +1129,11 @@
       <c r="Q7">
         <v>6</v>
       </c>
-      <c r="R7"/>
-    </row>
-    <row r="8" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="R7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1137,9 +1172,12 @@
       <c r="Q8">
         <v>999</v>
       </c>
-      <c r="R8"/>
-    </row>
-    <row r="9" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="R8" s="1">
+        <v>6</v>
+      </c>
+      <c r="S8"/>
+    </row>
+    <row r="9" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1188,9 +1226,12 @@
       <c r="Q9">
         <v>0</v>
       </c>
-      <c r="R9"/>
-    </row>
-    <row r="10" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="R9" s="1">
+        <v>7</v>
+      </c>
+      <c r="S9"/>
+    </row>
+    <row r="10" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1236,9 +1277,12 @@
       <c r="Q10">
         <v>10</v>
       </c>
-      <c r="R10"/>
-    </row>
-    <row r="11" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="R10" s="1">
+        <v>8</v>
+      </c>
+      <c r="S10"/>
+    </row>
+    <row r="11" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1277,7 +1321,10 @@
       <c r="Q11">
         <v>1000</v>
       </c>
-      <c r="R11"/>
+      <c r="R11" s="1">
+        <v>9</v>
+      </c>
+      <c r="S11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modified example_sblar.xlsx to fix merger conflict
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sultanin/Workspace/git/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A0E86B-2EE7-9045-9D1E-5FF5FF068522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DAEF69-B113-894F-ACB5-0E43DEF106C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="48">
   <si>
     <t>uid</t>
   </si>
@@ -748,10 +748,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -769,7 +769,7 @@
     <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -818,14 +818,17 @@
       <c r="P1" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" t="s">
         <v>43</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -869,14 +872,17 @@
         <v>1</v>
       </c>
       <c r="P2"/>
-      <c r="Q2" s="1">
+      <c r="Q2">
         <v>1</v>
       </c>
       <c r="R2" s="1">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -919,14 +925,17 @@
         <v>101</v>
       </c>
       <c r="P3"/>
-      <c r="Q3" s="1">
+      <c r="Q3">
         <v>2</v>
       </c>
       <c r="R3" s="1">
+        <v>2</v>
+      </c>
+      <c r="S3" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -966,14 +975,17 @@
         <v>1</v>
       </c>
       <c r="P4"/>
-      <c r="Q4" s="1">
+      <c r="Q4">
         <v>3</v>
       </c>
       <c r="R4" s="1">
+        <v>3</v>
+      </c>
+      <c r="S4" s="1">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1019,14 +1031,17 @@
         <v>102</v>
       </c>
       <c r="P5"/>
-      <c r="Q5" s="1">
+      <c r="Q5">
         <v>4</v>
       </c>
       <c r="R5" s="1">
+        <v>4</v>
+      </c>
+      <c r="S5" s="1">
         <v>12.5</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1071,14 +1086,17 @@
         <v>39</v>
       </c>
       <c r="P6"/>
-      <c r="Q6" s="1">
+      <c r="Q6">
         <v>5</v>
       </c>
       <c r="R6" s="1">
+        <v>5</v>
+      </c>
+      <c r="S6" s="1">
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1114,14 +1132,17 @@
         <v>999</v>
       </c>
       <c r="P7"/>
-      <c r="Q7" s="1">
+      <c r="Q7">
         <v>6</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="R7" s="1">
+        <v>6</v>
+      </c>
+      <c r="S7" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1157,14 +1178,17 @@
         <v>40</v>
       </c>
       <c r="P8"/>
-      <c r="Q8" s="1">
+      <c r="Q8">
+        <v>999</v>
+      </c>
+      <c r="R8" s="1">
         <v>7</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1210,14 +1234,17 @@
       <c r="P9" t="s">
         <v>41</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1">
         <v>900</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1260,14 +1287,17 @@
         <v>42</v>
       </c>
       <c r="P10"/>
-      <c r="Q10" s="1">
-        <v>1</v>
+      <c r="Q10">
+        <v>10</v>
       </c>
       <c r="R10" s="1">
+        <v>1</v>
+      </c>
+      <c r="S10" s="1">
         <v>3.4</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1303,10 +1333,13 @@
         <v>977</v>
       </c>
       <c r="P11"/>
-      <c r="Q11" s="1">
+      <c r="Q11">
+        <v>1000</v>
+      </c>
+      <c r="R11" s="1">
         <v>3</v>
       </c>
-      <c r="R11" s="1">
+      <c r="S11" s="1">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified example_sblar.xlsx to fix merge conflict
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sultanin/Workspace/git/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FD6679-DA64-E141-A737-B0C39EE0D801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3885AB-DCEC-D74A-8D11-A5550C2B0C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5640" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
   <sheets>
     <sheet name="valid" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
   <si>
     <t>uid</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>1;3;4;999</t>
+  </si>
+  <si>
+    <t>pricing_interest_rate_type</t>
   </si>
   <si>
     <t>pricing_prepenalty_allowed</t>
@@ -739,10 +742,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -757,10 +760,13 @@
     <col min="8" max="8" width="14.5" style="1" customWidth="1"/>
     <col min="9" max="11" width="10.83203125" style="1"/>
     <col min="12" max="12" width="19" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="1"/>
+    <col min="13" max="16" width="10.83203125" style="1"/>
+    <col min="17" max="17" width="22.33203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14.83203125" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -809,14 +815,17 @@
       <c r="P1" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -860,14 +869,17 @@
         <v>1</v>
       </c>
       <c r="P2"/>
-      <c r="Q2" s="1">
-        <v>1</v>
-      </c>
-      <c r="R2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -910,14 +922,17 @@
         <v>101</v>
       </c>
       <c r="P3"/>
-      <c r="Q3" s="1">
-        <v>2</v>
-      </c>
-      <c r="R3" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
+        <v>2</v>
+      </c>
+      <c r="S3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -957,14 +972,17 @@
         <v>1</v>
       </c>
       <c r="P4"/>
-      <c r="Q4" s="1">
+      <c r="Q4">
+        <v>3</v>
+      </c>
+      <c r="R4">
         <v>999</v>
       </c>
-      <c r="R4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1010,14 +1028,17 @@
         <v>102</v>
       </c>
       <c r="P5"/>
-      <c r="Q5" s="1">
+      <c r="Q5">
+        <v>4</v>
+      </c>
+      <c r="R5">
         <v>0</v>
       </c>
-      <c r="R5" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1062,14 +1083,17 @@
         <v>39</v>
       </c>
       <c r="P6"/>
-      <c r="Q6" s="1">
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6">
         <v>3</v>
       </c>
-      <c r="R6" s="1">
+      <c r="S6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1105,14 +1129,17 @@
         <v>999</v>
       </c>
       <c r="P7"/>
-      <c r="Q7" s="1">
-        <v>1</v>
-      </c>
-      <c r="R7" s="1">
+      <c r="Q7">
+        <v>6</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1148,14 +1175,17 @@
         <v>40</v>
       </c>
       <c r="P8"/>
-      <c r="Q8" s="1">
-        <v>2</v>
-      </c>
-      <c r="R8" s="1">
+      <c r="Q8">
         <v>999</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="R8">
+        <v>2</v>
+      </c>
+      <c r="S8">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1201,14 +1231,17 @@
       <c r="P9" t="s">
         <v>41</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
         <v>999</v>
       </c>
-      <c r="R9" s="1">
+      <c r="S9">
         <v>999</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1251,14 +1284,17 @@
         <v>42</v>
       </c>
       <c r="P10"/>
-      <c r="Q10" s="1">
+      <c r="Q10">
+        <v>10</v>
+      </c>
+      <c r="R10">
         <v>0</v>
       </c>
-      <c r="R10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1294,10 +1330,13 @@
         <v>977</v>
       </c>
       <c r="P11"/>
-      <c r="Q11" s="1">
+      <c r="Q11">
+        <v>1000</v>
+      </c>
+      <c r="R11">
         <v>0</v>
       </c>
-      <c r="R11" s="1">
+      <c r="S11">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add pricing_penalty_allowed and pricing_penalty_exits fields to example_sblar.xlsx and changed function name is_numeric_format to is_number in check_functions.py and schema.py
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sultanin/Workspace/git/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2A142B-F4AA-5C4B-9CB9-501FB8CF973E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82650FF-E157-644A-BEBE-B9E7C40C1BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>uid</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>pricing_init_rate_period</t>
+  </si>
+  <si>
+    <t>pricing_prepenalty_allowed</t>
+  </si>
+  <si>
+    <t>pricing_prepenalty_exists</t>
   </si>
 </sst>
 </file>
@@ -739,10 +745,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -763,7 +769,7 @@
     <col min="19" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -818,8 +824,14 @@
       <c r="R1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S1" t="s">
+        <v>45</v>
+      </c>
+      <c r="T1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -869,8 +881,14 @@
       <c r="R2">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -919,8 +937,14 @@
       <c r="R3">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S3">
+        <v>2</v>
+      </c>
+      <c r="T3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -966,8 +990,14 @@
       <c r="R4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S4">
+        <v>999</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1019,8 +1049,14 @@
       <c r="R5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1071,8 +1107,14 @@
       <c r="R6">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S6">
+        <v>3</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1114,8 +1156,14 @@
       <c r="R7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1157,8 +1205,14 @@
       <c r="R8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S8">
+        <v>2</v>
+      </c>
+      <c r="T8">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1210,8 +1264,14 @@
       <c r="R9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S9">
+        <v>999</v>
+      </c>
+      <c r="T9">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1258,8 +1318,14 @@
         <v>10</v>
       </c>
       <c r="R10"/>
-    </row>
-    <row r="11" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1300,6 +1366,12 @@
       </c>
       <c r="R11">
         <v>7</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated spreadsheet with values from main
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcguffeej/Documents/Projects/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9FCD82-FEE1-1848-95C5-AF8E21510A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC26BD66-59DA-B24E-9031-87F6DE53700C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t>uid</t>
   </si>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>pricing_var_margin</t>
+  </si>
+  <si>
+    <t>pricing_init_rate_period</t>
+  </si>
+  <si>
+    <t>pricing_prepenalty_allowed</t>
+  </si>
+  <si>
+    <t>pricing_prepenalty_exists</t>
   </si>
 </sst>
 </file>
@@ -742,10 +751,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -762,13 +771,15 @@
     <col min="12" max="12" width="19" style="1" customWidth="1"/>
     <col min="13" max="16" width="10.83203125" style="1"/>
     <col min="17" max="17" width="22.33203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="16.5" style="1" customWidth="1"/>
+    <col min="18" max="18" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17.5" style="1" customWidth="1"/>
     <col min="20" max="20" width="18" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="10.83203125" style="1"/>
+    <col min="21" max="21" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -820,14 +831,23 @@
       <c r="Q1" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="U1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -874,11 +894,20 @@
       <c r="Q2">
         <v>1</v>
       </c>
-      <c r="S2" t="s">
+      <c r="R2">
+        <v>24</v>
+      </c>
+      <c r="T2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -924,14 +953,23 @@
       <c r="Q3">
         <v>2</v>
       </c>
-      <c r="R3" t="s">
-        <v>41</v>
+      <c r="R3">
+        <v>36</v>
       </c>
       <c r="S3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="T3" t="s">
+        <v>41</v>
+      </c>
+      <c r="U3">
+        <v>2</v>
+      </c>
+      <c r="V3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -974,14 +1012,23 @@
       <c r="Q4">
         <v>3</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4" t="s">
         <v>41</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="U4">
+        <v>999</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1031,13 +1078,22 @@
         <v>4</v>
       </c>
       <c r="R5">
+        <v>2</v>
+      </c>
+      <c r="S5">
         <v>0</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1086,13 +1142,22 @@
         <v>5</v>
       </c>
       <c r="R6">
+        <v>2.5</v>
+      </c>
+      <c r="S6">
         <v>0.1</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="U6">
+        <v>3</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1132,10 +1197,19 @@
         <v>6</v>
       </c>
       <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1174,9 +1248,18 @@
       <c r="Q8">
         <v>999</v>
       </c>
-      <c r="S8"/>
-    </row>
-    <row r="9" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="T8"/>
+      <c r="U8">
+        <v>2</v>
+      </c>
+      <c r="V8">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1225,8 +1308,17 @@
       <c r="Q9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="R9">
+        <v>5</v>
+      </c>
+      <c r="U9">
+        <v>999</v>
+      </c>
+      <c r="V9">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1272,8 +1364,15 @@
       <c r="Q10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="R10"/>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1311,6 +1410,15 @@
       <c r="P11"/>
       <c r="Q11">
         <v>1000</v>
+      </c>
+      <c r="R11">
+        <v>7</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pricing_origination_charges, pricing_broker_fees, and pricing_initial_charges fields  (#28)
Add validation(s) for pricing_origination_charges, pricing_broker_fees, and pricing_initial_charges fields
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sultanin/Workspace/git/pandera-parser-poc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harjatia/Projects/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82650FF-E157-644A-BEBE-B9E7C40C1BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C3B410-F4F0-824D-99AF-D6154627F111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
   <si>
     <t>uid</t>
   </si>
@@ -166,6 +166,27 @@
   </si>
   <si>
     <t>1;3;4;999</t>
+  </si>
+  <si>
+    <t>pricing_origination_charges</t>
+  </si>
+  <si>
+    <t>pricing_broker_fees</t>
+  </si>
+  <si>
+    <t>pricing_initial_charges</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
   </si>
   <si>
     <t>pricing_interest_rate_type</t>
@@ -745,10 +766,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:T11"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -763,13 +784,14 @@
     <col min="8" max="8" width="14.5" style="1" customWidth="1"/>
     <col min="9" max="11" width="10.83203125" style="1"/>
     <col min="12" max="12" width="19" style="1" customWidth="1"/>
-    <col min="13" max="16" width="10.83203125" style="1"/>
-    <col min="17" max="17" width="22.33203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="14.83203125" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" style="1"/>
+    <col min="13" max="15" width="10.83203125" style="1"/>
+    <col min="16" max="17" width="19.6640625" style="1" customWidth="1"/>
+    <col min="18" max="19" width="10.83203125" style="1"/>
+    <col min="20" max="20" width="21.5" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -819,19 +841,28 @@
         <v>38</v>
       </c>
       <c r="Q1" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R1" t="s">
+      <c r="V1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S1" t="s">
+      <c r="W1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -887,8 +918,17 @@
       <c r="T2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U2" s="1">
+        <v>1</v>
+      </c>
+      <c r="V2" s="1">
+        <v>6</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -943,8 +983,17 @@
       <c r="T3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U3" s="1">
+        <v>2</v>
+      </c>
+      <c r="V3" s="1">
+        <v>5</v>
+      </c>
+      <c r="W3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -996,8 +1045,17 @@
       <c r="T4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1055,8 +1113,17 @@
       <c r="T5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U5" s="1">
+        <v>4</v>
+      </c>
+      <c r="V5" s="1">
+        <v>5</v>
+      </c>
+      <c r="W5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1113,8 +1180,17 @@
       <c r="T6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U6" s="1">
+        <v>5</v>
+      </c>
+      <c r="V6" s="1">
+        <v>5</v>
+      </c>
+      <c r="W6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1162,8 +1238,17 @@
       <c r="T7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U7" s="1">
+        <v>6</v>
+      </c>
+      <c r="V7" s="1">
+        <v>5</v>
+      </c>
+      <c r="W7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1211,8 +1296,17 @@
       <c r="T8">
         <v>999</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V8" s="1">
+        <v>5</v>
+      </c>
+      <c r="W8" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1270,8 +1364,17 @@
       <c r="T9">
         <v>999</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U9" s="1">
+        <v>8</v>
+      </c>
+      <c r="V9" s="1">
+        <v>5</v>
+      </c>
+      <c r="W9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1324,8 +1427,17 @@
       <c r="T10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="U10" s="1">
+        <v>8</v>
+      </c>
+      <c r="V10" s="1">
+        <v>5</v>
+      </c>
+      <c r="W10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1371,6 +1483,15 @@
         <v>0</v>
       </c>
       <c r="T11">
+        <v>2</v>
+      </c>
+      <c r="U11" s="1">
+        <v>10</v>
+      </c>
+      <c r="V11" s="1">
+        <v>5</v>
+      </c>
+      <c r="W11" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update excel from main
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcguffeej/Documents/Projects/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC26BD66-59DA-B24E-9031-87F6DE53700C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE019A9-3180-CB45-88A3-BCB8FE357AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
   <si>
     <t>uid</t>
   </si>
@@ -184,6 +184,27 @@
   </si>
   <si>
     <t>pricing_prepenalty_exists</t>
+  </si>
+  <si>
+    <t>pricing_origination_charges</t>
+  </si>
+  <si>
+    <t>pricing_broker_fees</t>
+  </si>
+  <si>
+    <t>pricing_initial_charges</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
   </si>
 </sst>
 </file>
@@ -751,10 +772,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:V11"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -776,10 +797,13 @@
     <col min="20" max="20" width="18" style="1" customWidth="1"/>
     <col min="21" max="21" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="10.83203125" style="1"/>
+    <col min="23" max="23" width="19.83203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -840,14 +864,23 @@
       <c r="T1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="X1" t="s">
         <v>47</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -900,14 +933,23 @@
       <c r="T2" t="s">
         <v>41</v>
       </c>
-      <c r="U2">
-        <v>1</v>
-      </c>
-      <c r="V2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="U2" s="1">
+        <v>1</v>
+      </c>
+      <c r="V2" s="1">
+        <v>6</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -962,14 +1004,23 @@
       <c r="T3" t="s">
         <v>41</v>
       </c>
-      <c r="U3">
-        <v>2</v>
-      </c>
-      <c r="V3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="U3" s="1">
+        <v>2</v>
+      </c>
+      <c r="V3" s="1">
+        <v>5</v>
+      </c>
+      <c r="W3" s="1">
+        <v>2</v>
+      </c>
+      <c r="X3">
+        <v>2</v>
+      </c>
+      <c r="Y3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1021,14 +1072,23 @@
       <c r="T4">
         <v>0</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="X4">
         <v>999</v>
       </c>
-      <c r="V4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="Y4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1086,14 +1146,23 @@
       <c r="T5">
         <v>0.1</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="1">
+        <v>4</v>
+      </c>
+      <c r="V5" s="1">
+        <v>5</v>
+      </c>
+      <c r="W5" s="1">
+        <v>2</v>
+      </c>
+      <c r="X5">
         <v>0</v>
       </c>
-      <c r="V5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="Y5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1150,14 +1219,23 @@
       <c r="T6">
         <v>0.2</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="1">
+        <v>5</v>
+      </c>
+      <c r="V6" s="1">
+        <v>5</v>
+      </c>
+      <c r="W6" s="1">
+        <v>2</v>
+      </c>
+      <c r="X6">
         <v>3</v>
       </c>
-      <c r="V6">
+      <c r="Y6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1202,14 +1280,23 @@
       <c r="S7">
         <v>0.2</v>
       </c>
-      <c r="U7">
-        <v>1</v>
-      </c>
-      <c r="V7">
+      <c r="U7" s="1">
+        <v>6</v>
+      </c>
+      <c r="V7" s="1">
+        <v>5</v>
+      </c>
+      <c r="W7" s="1">
+        <v>2</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="Y7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1252,14 +1339,23 @@
         <v>1</v>
       </c>
       <c r="T8"/>
-      <c r="U8">
-        <v>2</v>
-      </c>
-      <c r="V8">
+      <c r="U8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V8" s="1">
+        <v>5</v>
+      </c>
+      <c r="W8" s="1">
+        <v>22</v>
+      </c>
+      <c r="X8">
+        <v>2</v>
+      </c>
+      <c r="Y8">
         <v>999</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1311,14 +1407,23 @@
       <c r="R9">
         <v>5</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="1">
+        <v>8</v>
+      </c>
+      <c r="V9" s="1">
+        <v>5</v>
+      </c>
+      <c r="W9" s="1">
+        <v>2</v>
+      </c>
+      <c r="X9">
         <v>999</v>
       </c>
-      <c r="V9">
+      <c r="Y9">
         <v>999</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1365,14 +1470,23 @@
         <v>10</v>
       </c>
       <c r="R10"/>
-      <c r="U10">
+      <c r="U10" s="1">
+        <v>8</v>
+      </c>
+      <c r="V10" s="1">
+        <v>5</v>
+      </c>
+      <c r="W10" s="1">
+        <v>2</v>
+      </c>
+      <c r="X10">
         <v>0</v>
       </c>
-      <c r="V10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+      <c r="Y10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1414,10 +1528,19 @@
       <c r="R11">
         <v>7</v>
       </c>
-      <c r="U11">
+      <c r="U11" s="1">
+        <v>10</v>
+      </c>
+      <c r="V11" s="1">
+        <v>5</v>
+      </c>
+      <c r="W11" s="1">
+        <v>2</v>
+      </c>
+      <c r="X11">
         <v>0</v>
       </c>
-      <c r="V11">
+      <c r="Y11">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added bad data to example_sblar.xlsx
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harjatia/Projects/pandera-parser-poc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bienstocke/Documents/Github/columnar-SBLAR-parser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C3B410-F4F0-824D-99AF-D6154627F111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCE74FE-A25D-6F4E-A49C-95DC9484A3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
+    <workbookView xWindow="29180" yWindow="500" windowWidth="40320" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
   <sheets>
     <sheet name="valid" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="58">
   <si>
     <t>uid</t>
   </si>
@@ -199,6 +199,18 @@
   </si>
   <si>
     <t>pricing_prepenalty_exists</t>
+  </si>
+  <si>
+    <t>pricing_var_index_name</t>
+  </si>
+  <si>
+    <t>pricing_var_index_name_ff</t>
+  </si>
+  <si>
+    <t>What does this do if pricing_var_index_name has an invalid value?</t>
+  </si>
+  <si>
+    <t>Should be blank</t>
   </si>
 </sst>
 </file>
@@ -579,7 +591,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection sqref="A1:E11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -766,10 +778,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -788,10 +800,14 @@
     <col min="16" max="17" width="19.6640625" style="1" customWidth="1"/>
     <col min="18" max="19" width="10.83203125" style="1"/>
     <col min="20" max="20" width="21.5" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="10.83203125" style="1"/>
+    <col min="21" max="21" width="31.6640625" style="1" customWidth="1"/>
+    <col min="22" max="23" width="10.83203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="26" style="1" customWidth="1"/>
+    <col min="25" max="25" width="30.6640625" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -861,8 +877,14 @@
       <c r="W1" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="X1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -927,8 +949,14 @@
       <c r="W2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="X2" s="1">
+        <v>11</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -992,8 +1020,11 @@
       <c r="W3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="X3" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1054,8 +1085,11 @@
       <c r="W4" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="X4" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1122,8 +1156,11 @@
       <c r="W5" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="X5" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1189,8 +1226,11 @@
       <c r="W6" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="X6" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1247,8 +1287,11 @@
       <c r="W7" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="X7" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1305,8 +1348,11 @@
       <c r="W8" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="X8" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1373,8 +1419,11 @@
       <c r="W9" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="X9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1436,8 +1485,11 @@
       <c r="W10" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="X10" s="1">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1493,6 +1545,12 @@
       </c>
       <c r="W11" s="1">
         <v>2</v>
+      </c>
+      <c r="X11" s="1">
+        <v>999</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated spreadsheet with vals from main
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bienstocke/Documents/Github/columnar-SBLAR-parser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcguffeej/Documents/Projects/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCE74FE-A25D-6F4E-A49C-95DC9484A3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FB18DE-E48E-6445-A3BE-209EE7DA0639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29180" yWindow="500" windowWidth="40320" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
   <sheets>
     <sheet name="valid" sheetId="1" r:id="rId1"/>
@@ -591,7 +591,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -780,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="Y11" sqref="Y11"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -800,11 +800,11 @@
     <col min="16" max="17" width="19.6640625" style="1" customWidth="1"/>
     <col min="18" max="19" width="10.83203125" style="1"/>
     <col min="20" max="20" width="21.5" style="1" customWidth="1"/>
-    <col min="21" max="21" width="31.6640625" style="1" customWidth="1"/>
-    <col min="22" max="23" width="10.83203125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="26" style="1" customWidth="1"/>
-    <col min="25" max="25" width="30.6640625" style="1" customWidth="1"/>
-    <col min="26" max="16384" width="10.83203125" style="1"/>
+    <col min="21" max="21" width="24" style="1" customWidth="1"/>
+    <col min="22" max="22" width="23.33203125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="23.6640625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="19.1640625" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="51" x14ac:dyDescent="0.2">
@@ -869,22 +869,22 @@
         <v>53</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:25" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -941,19 +941,19 @@
         <v>1</v>
       </c>
       <c r="U2" s="1">
-        <v>1</v>
-      </c>
-      <c r="V2" s="1">
+        <v>11</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1</v>
+      </c>
+      <c r="X2" s="1">
         <v>6</v>
       </c>
-      <c r="W2" s="1">
-        <v>1</v>
-      </c>
-      <c r="X2" s="1">
-        <v>11</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>56</v>
+      <c r="Y2" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="17" x14ac:dyDescent="0.2">
@@ -1012,16 +1012,16 @@
         <v>2</v>
       </c>
       <c r="U3" s="1">
-        <v>2</v>
-      </c>
-      <c r="V3" s="1">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="W3" s="1">
         <v>2</v>
       </c>
       <c r="X3" s="1">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="17" x14ac:dyDescent="0.2">
@@ -1076,17 +1076,17 @@
       <c r="T4">
         <v>1</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="U4" s="1">
+        <v>13</v>
+      </c>
+      <c r="W4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="Y4" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="X4" s="1">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="17" x14ac:dyDescent="0.2">
@@ -1148,16 +1148,16 @@
         <v>2</v>
       </c>
       <c r="U5" s="1">
+        <v>14</v>
+      </c>
+      <c r="W5" s="1">
         <v>4</v>
       </c>
-      <c r="V5" s="1">
-        <v>5</v>
-      </c>
-      <c r="W5" s="1">
-        <v>2</v>
-      </c>
       <c r="X5" s="1">
-        <v>14</v>
+        <v>5</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="17" x14ac:dyDescent="0.2">
@@ -1218,16 +1218,16 @@
         <v>0</v>
       </c>
       <c r="U6" s="1">
-        <v>5</v>
-      </c>
-      <c r="V6" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="W6" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="X6" s="1">
-        <v>15</v>
+        <v>5</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="17" x14ac:dyDescent="0.2">
@@ -1279,16 +1279,16 @@
         <v>0</v>
       </c>
       <c r="U7" s="1">
+        <v>16</v>
+      </c>
+      <c r="W7" s="1">
         <v>6</v>
       </c>
-      <c r="V7" s="1">
-        <v>5</v>
-      </c>
-      <c r="W7" s="1">
-        <v>2</v>
-      </c>
       <c r="X7" s="1">
-        <v>16</v>
+        <v>5</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="17" x14ac:dyDescent="0.2">
@@ -1339,17 +1339,17 @@
       <c r="T8">
         <v>999</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="U8" s="1">
+        <v>17</v>
+      </c>
+      <c r="W8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="V8" s="1">
-        <v>5</v>
-      </c>
-      <c r="W8" s="1">
+      <c r="X8" s="1">
+        <v>5</v>
+      </c>
+      <c r="Y8" s="1">
         <v>22</v>
-      </c>
-      <c r="X8" s="1">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="17" x14ac:dyDescent="0.2">
@@ -1411,16 +1411,16 @@
         <v>999</v>
       </c>
       <c r="U9" s="1">
+        <v>1</v>
+      </c>
+      <c r="W9" s="1">
         <v>8</v>
       </c>
-      <c r="V9" s="1">
-        <v>5</v>
-      </c>
-      <c r="W9" s="1">
-        <v>2</v>
-      </c>
       <c r="X9" s="1">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="17" x14ac:dyDescent="0.2">
@@ -1477,19 +1477,19 @@
         <v>1</v>
       </c>
       <c r="U10" s="1">
+        <v>977</v>
+      </c>
+      <c r="W10" s="1">
         <v>8</v>
       </c>
-      <c r="V10" s="1">
-        <v>5</v>
-      </c>
-      <c r="W10" s="1">
-        <v>2</v>
-      </c>
       <c r="X10" s="1">
-        <v>977</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1538,19 +1538,19 @@
         <v>2</v>
       </c>
       <c r="U11" s="1">
+        <v>999</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="W11" s="1">
         <v>10</v>
       </c>
-      <c r="V11" s="1">
-        <v>5</v>
-      </c>
-      <c r="W11" s="1">
-        <v>2</v>
-      </c>
       <c r="X11" s="1">
-        <v>999</v>
-      </c>
-      <c r="Y11" s="1" t="s">
-        <v>57</v>
+        <v>5</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Task 555 - added validation for gross_annual_revenue and gross_annual_revenue_flag fields
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harjatia/Projects/pandera-parser-poc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sultanin/Workspace/git/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C3B410-F4F0-824D-99AF-D6154627F111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E6D369-F333-9846-BBC9-83F29CEF6A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
+    <workbookView xWindow="400" yWindow="3600" windowWidth="33600" windowHeight="18800" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
   <sheets>
     <sheet name="valid" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
   <si>
     <t>uid</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>pricing_prepenalty_exists</t>
+  </si>
+  <si>
+    <t>gross_annual_revenue_flag</t>
+  </si>
+  <si>
+    <t>gross_annual_revenue</t>
   </si>
 </sst>
 </file>
@@ -766,10 +772,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -791,7 +797,7 @@
     <col min="21" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -861,8 +867,14 @@
       <c r="W1" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="X1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -927,8 +939,14 @@
       <c r="W2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="X2" s="1">
+        <v>900</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -992,8 +1010,11 @@
       <c r="W3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="X3" s="1">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1054,8 +1075,11 @@
       <c r="W4" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="X4" s="1">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1122,8 +1146,14 @@
       <c r="W5" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="X5" s="1">
+        <v>988</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1189,8 +1219,11 @@
       <c r="W6" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="Y6" s="1">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1247,8 +1280,11 @@
       <c r="W7" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="X7" s="1">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1305,8 +1341,14 @@
       <c r="W8" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="X8" s="1">
+        <v>990</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1373,8 +1415,14 @@
       <c r="W9" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="X9" s="1">
+        <v>900</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1436,8 +1484,11 @@
       <c r="W10" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+      <c r="X10" s="1">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1493,6 +1544,12 @@
       </c>
       <c r="W11" s="1">
         <v>2</v>
+      </c>
+      <c r="X11" s="1">
+        <v>900</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>50000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add number_of_workers validation (#40)
* add number_of_workers validation

* updated to match main branch new function names
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcguffeej/Documents/Projects/pandera-parser-poc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harjatia/Projects/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FB18DE-E48E-6445-A3BE-209EE7DA0639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8BC760-6B9E-994B-96DC-5097CEE77BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
+    <workbookView xWindow="-300" yWindow="4120" windowWidth="33600" windowHeight="19040" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
   <sheets>
     <sheet name="valid" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
   <si>
     <t>uid</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>Should be blank</t>
+  </si>
+  <si>
+    <t>number_of_workers</t>
   </si>
 </sst>
 </file>
@@ -591,7 +594,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection sqref="A1:E11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -778,10 +781,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:Y11"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -800,14 +803,14 @@
     <col min="16" max="17" width="19.6640625" style="1" customWidth="1"/>
     <col min="18" max="19" width="10.83203125" style="1"/>
     <col min="20" max="20" width="21.5" style="1" customWidth="1"/>
-    <col min="21" max="21" width="24" style="1" customWidth="1"/>
-    <col min="22" max="22" width="23.33203125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="23.6640625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="19.1640625" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="10.83203125" style="1"/>
+    <col min="21" max="21" width="31.6640625" style="1" customWidth="1"/>
+    <col min="22" max="23" width="10.83203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="26" style="1" customWidth="1"/>
+    <col min="25" max="25" width="30.6640625" style="1" customWidth="1"/>
+    <col min="26" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -869,22 +872,25 @@
         <v>53</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" ht="119" x14ac:dyDescent="0.2">
+      <c r="Z1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -941,22 +947,25 @@
         <v>1</v>
       </c>
       <c r="U2" s="1">
+        <v>1</v>
+      </c>
+      <c r="V2" s="1">
+        <v>6</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1</v>
+      </c>
+      <c r="X2" s="1">
         <v>11</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="W2" s="1">
-        <v>1</v>
-      </c>
-      <c r="X2" s="1">
-        <v>6</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="Z2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1012,19 +1021,22 @@
         <v>2</v>
       </c>
       <c r="U3" s="1">
+        <v>2</v>
+      </c>
+      <c r="V3" s="1">
+        <v>5</v>
+      </c>
+      <c r="W3" s="1">
+        <v>2</v>
+      </c>
+      <c r="X3" s="1">
         <v>12</v>
       </c>
-      <c r="W3" s="1">
-        <v>2</v>
-      </c>
-      <c r="X3" s="1">
-        <v>5</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="Z3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1076,20 +1088,23 @@
       <c r="T4">
         <v>1</v>
       </c>
-      <c r="U4" s="1">
+      <c r="U4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X4" s="1">
         <v>13</v>
       </c>
-      <c r="W4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="Z4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1148,19 +1163,22 @@
         <v>2</v>
       </c>
       <c r="U5" s="1">
+        <v>4</v>
+      </c>
+      <c r="V5" s="1">
+        <v>5</v>
+      </c>
+      <c r="W5" s="1">
+        <v>2</v>
+      </c>
+      <c r="X5" s="1">
         <v>14</v>
       </c>
-      <c r="W5" s="1">
+      <c r="Z5" s="1">
         <v>4</v>
       </c>
-      <c r="X5" s="1">
-        <v>5</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1218,19 +1236,22 @@
         <v>0</v>
       </c>
       <c r="U6" s="1">
+        <v>5</v>
+      </c>
+      <c r="V6" s="1">
+        <v>5</v>
+      </c>
+      <c r="W6" s="1">
+        <v>2</v>
+      </c>
+      <c r="X6" s="1">
         <v>15</v>
       </c>
-      <c r="W6" s="1">
-        <v>5</v>
-      </c>
-      <c r="X6" s="1">
-        <v>5</v>
-      </c>
-      <c r="Y6" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="Z6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1279,19 +1300,22 @@
         <v>0</v>
       </c>
       <c r="U7" s="1">
+        <v>6</v>
+      </c>
+      <c r="V7" s="1">
+        <v>5</v>
+      </c>
+      <c r="W7" s="1">
+        <v>2</v>
+      </c>
+      <c r="X7" s="1">
         <v>16</v>
       </c>
-      <c r="W7" s="1">
+      <c r="Z7" s="1">
         <v>6</v>
       </c>
-      <c r="X7" s="1">
-        <v>5</v>
-      </c>
-      <c r="Y7" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1339,20 +1363,23 @@
       <c r="T8">
         <v>999</v>
       </c>
-      <c r="U8" s="1">
+      <c r="U8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V8" s="1">
+        <v>5</v>
+      </c>
+      <c r="W8" s="1">
+        <v>22</v>
+      </c>
+      <c r="X8" s="1">
         <v>17</v>
       </c>
-      <c r="W8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="X8" s="1">
-        <v>5</v>
-      </c>
-      <c r="Y8" s="1">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+      <c r="Z8" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1411,19 +1438,22 @@
         <v>999</v>
       </c>
       <c r="U9" s="1">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="V9" s="1">
+        <v>5</v>
       </c>
       <c r="W9" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="X9" s="1">
-        <v>5</v>
-      </c>
-      <c r="Y9" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1477,19 +1507,19 @@
         <v>1</v>
       </c>
       <c r="U10" s="1">
+        <v>8</v>
+      </c>
+      <c r="V10" s="1">
+        <v>5</v>
+      </c>
+      <c r="W10" s="1">
+        <v>2</v>
+      </c>
+      <c r="X10" s="1">
         <v>977</v>
       </c>
-      <c r="W10" s="1">
-        <v>8</v>
-      </c>
-      <c r="X10" s="1">
-        <v>5</v>
-      </c>
-      <c r="Y10" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1538,19 +1568,22 @@
         <v>2</v>
       </c>
       <c r="U11" s="1">
+        <v>10</v>
+      </c>
+      <c r="V11" s="1">
+        <v>5</v>
+      </c>
+      <c r="W11" s="1">
+        <v>2</v>
+      </c>
+      <c r="X11" s="1">
         <v>999</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="Y11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="W11" s="1">
-        <v>10</v>
-      </c>
-      <c r="X11" s="1">
-        <v>5</v>
-      </c>
-      <c r="Y11" s="1">
-        <v>2</v>
+      <c r="Z11" s="1">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding gross_annual_revenue_flag and gross_annual_revenue fields to example_sblar.xlsx file
</commit_message>
<xml_diff>
--- a/example_sblar.xlsx
+++ b/example_sblar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sultanin/Workspace/git/pandera-parser-poc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64978F46-31C6-2F4D-BE3F-BA55AF6405F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCACDB6-DF4D-3B4F-B86E-EEF37FF6D40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1720" windowWidth="33600" windowHeight="19040" activeTab="1" xr2:uid="{4C11B797-997E-4D4A-9DAD-4BB9114BC471}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t>uid</t>
   </si>
@@ -214,6 +214,12 @@
   </si>
   <si>
     <t>number_of_workers</t>
+  </si>
+  <si>
+    <t>gross_annual_revenue_flag</t>
+  </si>
+  <si>
+    <t>gross_annual_revenue</t>
   </si>
 </sst>
 </file>
@@ -781,10 +787,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CC94F5-25C3-FC44-972B-B7BB739BAD9C}">
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:AB11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="Z14" sqref="Z14"/>
+      <selection activeCell="AA1" sqref="AA1:AB11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -810,7 +816,7 @@
     <col min="26" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -889,8 +895,14 @@
       <c r="Z1" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" ht="51" x14ac:dyDescent="0.2">
+      <c r="AA1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -964,8 +976,14 @@
       <c r="Z2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA2" s="1">
+        <v>900</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1035,8 +1053,11 @@
       <c r="Z3" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA3" s="1">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1103,8 +1124,11 @@
       <c r="Z4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA4" s="1">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1177,8 +1201,14 @@
       <c r="Z5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA5" s="1">
+        <v>988</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1250,8 +1280,11 @@
       <c r="Z6" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="AB6" s="1">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1314,8 +1347,11 @@
       <c r="Z7" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA7" s="1">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1378,8 +1414,14 @@
       <c r="Z8" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA8" s="1">
+        <v>990</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1452,8 +1494,14 @@
       <c r="Z9" s="1">
         <v>988</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA9" s="1">
+        <v>900</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1518,8 +1566,11 @@
       <c r="X10" s="1">
         <v>977</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+      <c r="AA10" s="1">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1584,6 +1635,12 @@
       </c>
       <c r="Z11" s="1">
         <v>12</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>900</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>50000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>